<commit_message>
complete reading and constructing problem
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onur\Dropbox\Dynamic Workforce Scheduling and Routing\MIP_Model_Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5DEA3A-4BBE-4688-9B9C-DA9E960494A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D1AA77-6552-4B6C-A862-4701D486E547}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9705" yWindow="1410" windowWidth="10470" windowHeight="7860" activeTab="1" xr2:uid="{860D2369-FF28-4586-B393-A17A06751C31}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{860D2369-FF28-4586-B393-A17A06751C31}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="5" r:id="rId1"/>
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE64BAA-DE87-45E2-BF66-4FA4CE157E2A}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D448B70-1AD1-4708-9485-F92A3B32F9F8}">
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2284,7 +2284,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>